<commit_message>
subindo atualizacao pre ultima aula
</commit_message>
<xml_diff>
--- a/projeto_final/model_out_corona.xlsx
+++ b/projeto_final/model_out_corona.xlsx
@@ -1,37 +1,162 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Desktop\python_aulas\projeto_final_3\PythonAulas\projeto_final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="analise_corona" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="analise_corona" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+  <si>
+    <t>Total de Casos</t>
+  </si>
+  <si>
+    <t>Novos Casos</t>
+  </si>
+  <si>
+    <t>Total de Mortes</t>
+  </si>
+  <si>
+    <t>Novas Mortes</t>
+  </si>
+  <si>
+    <t>Total de Recuperados</t>
+  </si>
+  <si>
+    <t>Casos Ativos</t>
+  </si>
+  <si>
+    <t>Sério ou Crítico</t>
+  </si>
+  <si>
+    <t>Total de Casos/1M População</t>
+  </si>
+  <si>
+    <t>Mortes/1M População</t>
+  </si>
+  <si>
+    <t>Total de Testes</t>
+  </si>
+  <si>
+    <t>Testes/1M População</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,10 +171,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -57,15 +190,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,1121 +495,1033 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total de Casos</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Novos Casos</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total de Mortes</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Novas Mortes</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total de Recuperados</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Casos Ativos</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Sério ou Crítico</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Total de Casos/1M População</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Mortes/1M População</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Total de Testes</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Testes/1M População</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
         <v>1526807</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>19034</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>90973</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>860</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>344933</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>1090901</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>16353</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>4616</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>275</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>11784538</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>35628</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>281752</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>9709</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2631</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>94</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>67373</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>211748</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>2300</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>1931</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>18</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>6916088</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>47394</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
         <v>277719</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>1214</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>27650</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>87</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>195945</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>54124</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>1152</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>5940</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>591</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>3037840</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>64977</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
         <v>243695</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>3534</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>34636</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>170</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5">
         <v>1559</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>3592</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5">
         <v>511</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>2580769</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5">
         <v>38041</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
         <v>241080</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>7938</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>16118</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>485</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>94122</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>130840</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>8318</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>1135</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>76</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>735224</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6">
         <v>3462</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
         <v>225435</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>675</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>31908</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>145</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>125176</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>68351</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>762</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>3728</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7">
         <v>528</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7">
         <v>3004960</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7">
         <v>49691</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
         <v>179569</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>204</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>28108</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>483</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>61213</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>90248</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>2087</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>2752</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8">
         <v>431</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8">
         <v>1384633</v>
       </c>
-      <c r="L8" t="n">
+      <c r="L8">
         <v>21218</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Germany</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
         <v>176651</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>407</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>8049</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>22</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>153400</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>15202</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>1166</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>2109</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9">
         <v>96</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9">
         <v>3147771</v>
       </c>
-      <c r="L9" t="n">
+      <c r="L9">
         <v>37585</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
         <v>149435</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>1368</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>4140</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>44</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>109962</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>35333</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>914</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>1774</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10">
         <v>49</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10">
         <v>1624994</v>
       </c>
-      <c r="L10" t="n">
+      <c r="L10">
         <v>19293</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Iran</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
         <v>120198</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>1806</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>6988</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>51</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>94464</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>18746</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>2705</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>1433</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11">
         <v>83</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11">
         <v>686935</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L11">
         <v>8192</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
         <v>95698</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>5050</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>3025</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>154</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>36795</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>55878</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>69</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12">
         <v>2</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12">
         <v>2227642</v>
       </c>
-      <c r="L12" t="n">
+      <c r="L12">
         <v>1616</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Peru</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
         <v>92273</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>3732</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>2648</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>125</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>28621</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>61004</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>850</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13">
         <v>2804</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13">
         <v>80</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13">
         <v>650613</v>
       </c>
-      <c r="L13" t="n">
+      <c r="L13">
         <v>19767</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>China</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
         <v>82947</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>4633</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>78227</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>87</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>10</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14">
         <v>58</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14">
         <v>3</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14">
         <v>0</v>
       </c>
-      <c r="L14" t="n">
+      <c r="L14">
         <v>0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
         <v>55280</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>291</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>9052</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>47</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>14630</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>31598</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>371</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15">
         <v>4772</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15">
         <v>781</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15">
         <v>682980</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L15">
         <v>58962</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Saudi Arabia</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
         <v>54752</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>2736</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>312</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>10</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>25722</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>28718</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>202</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16">
         <v>1576</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J16">
         <v>9</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K16">
         <v>586405</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L16">
         <v>16878</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Mexico</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
         <v>47144</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>2112</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>5045</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>278</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>31848</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>10251</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>378</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17">
         <v>366</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J17">
         <v>39</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K17">
         <v>163691</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L17">
         <v>1271</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
         <v>43995</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>125</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>5680</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>10</v>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18">
         <v>346</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18">
         <v>2568</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18">
         <v>332</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K18">
         <v>287943</v>
       </c>
-      <c r="L18" t="n">
+      <c r="L18">
         <v>16809</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Chile</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
         <v>43781</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>2353</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>450</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>29</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>19213</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>24118</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>769</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19">
         <v>2293</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19">
         <v>24</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K19">
         <v>363496</v>
       </c>
-      <c r="L19" t="n">
+      <c r="L19">
         <v>19035</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Pakistan</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
         <v>40151</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>1352</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>873</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>39</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>11341</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>27937</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>111</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20">
         <v>182</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20">
         <v>4</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K20">
         <v>373410</v>
       </c>
-      <c r="L20" t="n">
+      <c r="L20">
         <v>1695</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
         <v>33182</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>419</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>2736</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>48</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>3433</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>27013</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>189</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21">
         <v>1884</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21">
         <v>155</v>
       </c>
-      <c r="K21" t="n">
+      <c r="K21">
         <v>95047</v>
       </c>
-      <c r="L21" t="n">
+      <c r="L21">
         <v>5398</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Qatar</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
         <v>32604</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>1632</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>15</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>4370</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>28219</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>165</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22">
         <v>11341</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22">
         <v>5</v>
       </c>
-      <c r="K22" t="n">
+      <c r="K22">
         <v>157570</v>
       </c>
-      <c r="L22" t="n">
+      <c r="L22">
         <v>54811</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Switzerland</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
         <v>30587</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>15</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>1881</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>2</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>27500</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>1206</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>69</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23">
         <v>3537</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J23">
         <v>218</v>
       </c>
-      <c r="K23" t="n">
+      <c r="K23">
         <v>343359</v>
       </c>
-      <c r="L23" t="n">
+      <c r="L23">
         <v>39709</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Sweden</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
         <v>30143</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>466</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>3679</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>5</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>4971</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>21493</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>287</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24">
         <v>2987</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24">
         <v>365</v>
       </c>
-      <c r="K24" t="n">
+      <c r="K24">
         <v>177500</v>
       </c>
-      <c r="L24" t="n">
+      <c r="L24">
         <v>17589</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Belarus</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
         <v>29650</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>969</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>165</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>5</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>9932</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>19553</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25">
         <v>92</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25">
         <v>3138</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25">
         <v>17</v>
       </c>
-      <c r="K25" t="n">
+      <c r="K25">
         <v>350515</v>
       </c>
-      <c r="L25" t="n">
+      <c r="L25">
         <v>37093</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Portugal</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
         <v>29036</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>226</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>1218</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>15</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>4636</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>23182</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>108</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26">
         <v>2847</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26">
         <v>119</v>
       </c>
-      <c r="K26" t="n">
+      <c r="K26">
         <v>618066</v>
       </c>
-      <c r="L26" t="n">
+      <c r="L26">
         <v>60593</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Singapore</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
         <v>28038</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>682</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>22</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27">
         <v>0</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27">
         <v>9340</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27">
         <v>18676</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27">
         <v>16</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27">
         <v>4797</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27">
         <v>4</v>
       </c>
-      <c r="K27" t="n">
+      <c r="K27">
         <v>246254</v>
       </c>
-      <c r="L27" t="n">
+      <c r="L27">
         <v>42133</v>
       </c>
     </row>

</xml_diff>